<commit_message>
Complete SmartBlind testing on #21
</commit_message>
<xml_diff>
--- a/Firmware_Release/Zeus/Zeus_FW_SB430_3110_SS502_SC208.xlsx
+++ b/Firmware_Release/Zeus/Zeus_FW_SB430_3110_SS502_SC208.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\My Drive\001-Github\RYSE_Testing_record\Firmware_Release\Zeus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD87226-FC23-4FF6-B3D3-DECB6473FDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6043696-78DA-4CCA-84E1-198AD635A7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="9960" xr2:uid="{7785C230-C9C6-4B37-86E6-FED87339FA29}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7785C230-C9C6-4B37-86E6-FED87339FA29}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="184">
   <si>
     <t>Code</t>
   </si>
@@ -615,6 +615,12 @@
   </si>
   <si>
     <t>Check time error because using Canada's winter time</t>
+  </si>
+  <si>
+    <t>28-03-2025</t>
+  </si>
+  <si>
+    <t>FW_Android_App_Test_Suite_v1.7.4_CloudSyn_28Mar2024</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1283,7 @@
   <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1875,7 +1881,9 @@
       <c r="B43" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="11"/>
+      <c r="C43" s="11" t="s">
+        <v>182</v>
+      </c>
       <c r="D43" s="11" t="s">
         <v>23</v>
       </c>
@@ -1889,7 +1897,9 @@
       <c r="B44" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C44" s="8"/>
+      <c r="C44" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="D44" s="7" t="s">
         <v>23</v>
       </c>
@@ -1905,7 +1915,9 @@
       <c r="B45" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C45" s="20"/>
+      <c r="C45" s="20" t="s">
+        <v>182</v>
+      </c>
       <c r="D45" s="19" t="s">
         <v>23</v>
       </c>
@@ -1921,7 +1933,9 @@
       <c r="B46" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C46" s="8"/>
+      <c r="C46" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="D46" s="19" t="s">
         <v>23</v>
       </c>
@@ -1949,7 +1963,9 @@
       <c r="B48" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C48" s="8"/>
+      <c r="C48" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="D48" s="19" t="s">
         <v>23</v>
       </c>
@@ -1965,7 +1981,9 @@
       <c r="B49" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C49" s="20"/>
+      <c r="C49" s="20" t="s">
+        <v>182</v>
+      </c>
       <c r="D49" s="19" t="s">
         <v>23</v>
       </c>
@@ -1993,7 +2011,9 @@
       <c r="B51" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="C51" s="20"/>
+      <c r="C51" s="20" t="s">
+        <v>182</v>
+      </c>
       <c r="D51" s="19" t="s">
         <v>23</v>
       </c>
@@ -2011,7 +2031,9 @@
       <c r="B52" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C52" s="8"/>
+      <c r="C52" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="D52" s="19" t="s">
         <v>23</v>
       </c>
@@ -2198,7 +2220,9 @@
       <c r="B66" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C66" s="3"/>
+      <c r="C66" s="3" t="s">
+        <v>152</v>
+      </c>
       <c r="D66" s="2" t="s">
         <v>23</v>
       </c>
@@ -2224,7 +2248,9 @@
       <c r="B68" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C68" s="20"/>
+      <c r="C68" s="20" t="s">
+        <v>152</v>
+      </c>
       <c r="D68" s="19" t="s">
         <v>23</v>
       </c>
@@ -2240,7 +2266,9 @@
       <c r="B69" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C69" s="8"/>
+      <c r="C69" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="D69" s="19" t="s">
         <v>23</v>
       </c>
@@ -2256,7 +2284,9 @@
       <c r="B70" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="C70" s="26"/>
+      <c r="C70" s="26" t="s">
+        <v>152</v>
+      </c>
       <c r="D70" s="19" t="s">
         <v>23</v>
       </c>
@@ -2272,7 +2302,9 @@
       <c r="B71" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C71" s="8"/>
+      <c r="C71" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="D71" s="19" t="s">
         <v>23</v>
       </c>
@@ -2288,7 +2320,9 @@
       <c r="B72" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="C72" s="20"/>
+      <c r="C72" s="20" t="s">
+        <v>152</v>
+      </c>
       <c r="D72" s="19" t="s">
         <v>23</v>
       </c>
@@ -2303,7 +2337,9 @@
       <c r="B73" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C73" s="8"/>
+      <c r="C73" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="D73" s="19" t="s">
         <v>23</v>
       </c>
@@ -2321,7 +2357,9 @@
       <c r="B74" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="C74" s="20"/>
+      <c r="C74" s="20" t="s">
+        <v>152</v>
+      </c>
       <c r="D74" s="19" t="s">
         <v>23</v>
       </c>
@@ -2349,11 +2387,15 @@
       <c r="B77" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C77" s="3"/>
+      <c r="C77" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="D77" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E77" s="2"/>
+      <c r="E77" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2363,11 +2405,15 @@
       <c r="B78" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C78" s="8"/>
+      <c r="C78" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="D78" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E78" s="7"/>
+      <c r="E78" s="7" t="s">
+        <v>183</v>
+      </c>
       <c r="F78" s="7"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2377,11 +2423,15 @@
       <c r="B79" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C79" s="3"/>
+      <c r="C79" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="D79" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E79" s="2"/>
+      <c r="E79" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Finished IOS v2.3.1 app testing in tick #192
</commit_message>
<xml_diff>
--- a/Firmware_Release/Zeus/Zeus_FW_SB430_3110_SS502_SC208.xlsx
+++ b/Firmware_Release/Zeus/Zeus_FW_SB430_3110_SS502_SC208.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\My Drive\001-Github\RYSE_Testing_record\Firmware_Release\Zeus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6043696-78DA-4CCA-84E1-198AD635A7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CF6E8F-D962-4594-B3A9-70D531013BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7785C230-C9C6-4B37-86E6-FED87339FA29}"/>
   </bookViews>
@@ -1283,7 +1283,7 @@
   <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>